<commit_message>
updates to resolve comments in PR
</commit_message>
<xml_diff>
--- a/data-raw/R2R_TMH_habitat_inputs/River Length Summary.xlsx
+++ b/data-raw/R2R_TMH_habitat_inputs/River Length Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/R2R/DSMhabitat/data-raw/R2R_TMH_habitat_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E317B8-1546-7A43-AB60-D43FCA89B09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563C7B9D-1D96-3F48-89DA-1FACFCC3E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32960" yWindow="2080" windowWidth="28800" windowHeight="15760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1457,8 +1457,8 @@
   <dimension ref="A1:AA1061"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4032,7 +4032,9 @@
       <c r="F71" s="1">
         <v>122.45</v>
       </c>
-      <c r="I71" s="16"/>
+      <c r="I71" s="16">
+        <v>0</v>
+      </c>
       <c r="J71" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>